<commit_message>
Update test case : orderProduct - Add verify ordered-product on cart
</commit_message>
<xml_diff>
--- a/test-data/Product.xlsx
+++ b/test-data/Product.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="AddProduct" sheetId="1" r:id="rId1"/>
+    <sheet name="GuestUser" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Category</t>
   </si>
@@ -50,6 +51,99 @@
   </si>
   <si>
     <t>Basic No additional charge</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>DisplayedName</t>
+  </si>
+  <si>
+    <t>ConfirmPasswd</t>
+  </si>
+  <si>
+    <t>Passwd</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>State/Province</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>MobilePhone</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>thohip@gmail.com</t>
+  </si>
+  <si>
+    <t>ThoHip</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>HunterPro</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Phan</t>
+  </si>
+  <si>
+    <t>HCM123</t>
+  </si>
+  <si>
+    <t>00008</t>
+  </si>
+  <si>
+    <t>HCM</t>
+  </si>
+  <si>
+    <t>VietName</t>
+  </si>
+  <si>
+    <t>0979155626</t>
+  </si>
+  <si>
+    <t>Mrs</t>
   </si>
 </sst>
 </file>
@@ -108,11 +202,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,7 +515,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +546,7 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -465,7 +560,7 @@
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -476,4 +571,154 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="1">
+        <v>83123456</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
4. Open cart and do check out. -> Selenium script should verify what we’ve chosen 5. Fill some required information then check out as guest 6. Verify the inputted information and confirm purchase  -> Selenium script should verify our input information.
</commit_message>
<xml_diff>
--- a/test-data/Product.xlsx
+++ b/test-data/Product.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddProduct" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Category</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Address2</t>
   </si>
   <si>
-    <t>PostalCode</t>
-  </si>
-  <si>
     <t>City</t>
   </si>
   <si>
@@ -137,13 +134,19 @@
     <t>HCM</t>
   </si>
   <si>
-    <t>VietName</t>
-  </si>
-  <si>
     <t>0979155626</t>
   </si>
   <si>
     <t>Mrs</t>
+  </si>
+  <si>
+    <t>ZipCode</t>
+  </si>
+  <si>
+    <t>Viet Nam</t>
+  </si>
+  <si>
+    <t>83123456</t>
   </si>
 </sst>
 </file>
@@ -514,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,82 +643,82 @@
         <v>23</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1">
         <v>12345678</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" s="1">
-        <v>83123456</v>
+      <c r="S2" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>